<commit_message>
autocorrect I hate you
</commit_message>
<xml_diff>
--- a/files/Oros_Eng_Dictionary.xlsx
+++ b/files/Oros_Eng_Dictionary.xlsx
@@ -7161,7 +7161,7 @@
     <t xml:space="preserve">Nihongo</t>
   </si>
   <si>
-    <t xml:space="preserve">but</t>
+    <t xml:space="preserve">pus</t>
   </si>
   <si>
     <t xml:space="preserve">vulgar now; use 'ak' for chest</t>
@@ -16074,11 +16074,11 @@
   </sheetPr>
   <dimension ref="A1:Q1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A298" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L323" activeCellId="0" sqref="L323"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A443" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D466" activeCellId="0" sqref="D466"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.7734375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="0" width="8.5"/>

</xml_diff>

<commit_message>
hausa added - in progress
</commit_message>
<xml_diff>
--- a/files/Oros_Eng_Dictionary.xlsx
+++ b/files/Oros_Eng_Dictionary.xlsx
@@ -5622,10 +5622,10 @@
     <t xml:space="preserve">mek</t>
   </si>
   <si>
-    <t xml:space="preserve">creation/establishment/invention</t>
-  </si>
-  <si>
-    <t xml:space="preserve">make/create/manufacture/establish/invent</t>
+    <t xml:space="preserve">creation/good</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make/create/manufacture</t>
   </si>
   <si>
     <t xml:space="preserve">artificial</t>
@@ -14264,10 +14264,10 @@
     <t xml:space="preserve">inxiniy</t>
   </si>
   <si>
-    <t xml:space="preserve">innovation/creativity/originality/design/ingenuity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">innovate/create/design</t>
+    <t xml:space="preserve">innovation/creativity/originality/design/ingenuity/invention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">innovate/create/design/invent/establish</t>
   </si>
   <si>
     <t xml:space="preserve">creative/innovative/original/seminal/ingenious</t>
@@ -15918,8 +15918,8 @@
   </sheetPr>
   <dimension ref="A1:P1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A236" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F254" activeCellId="0" sqref="F254"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A345" colorId="64" zoomScale="81" zoomScaleNormal="81" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F367" activeCellId="0" sqref="F367"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.81640625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>